<commit_message>
updated rainfall data to include 2022, trying to figure out how to unscale my data
</commit_message>
<xml_diff>
--- a/raw/Rainfall.xlsx
+++ b/raw/Rainfall.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentstamuk-my.sharepoint.com/personal/joseph_hediger_students_tamuk_edu/Documents/Documents/1_R Projects/Survival/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\R Projects\Survival\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0A8F25A5-49AA-4BE5-9F16-9AF94B670FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA12E7C5-542F-47C4-9425-A4FE0F50A865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13728" yWindow="0" windowWidth="9408" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="16">
   <si>
     <t>EAST YANA</t>
   </si>
@@ -210,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +403,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -551,11 +570,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F248" sqref="F248"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="F252" sqref="F252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4229,17 +4249,17 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A237" s="1" t="s">
+      <c r="A237" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B237" s="3">
         <v>2021</v>
       </c>
       <c r="C237" s="2">
-        <v>5.9359999999999991</v>
+        <v>4</v>
       </c>
       <c r="D237" s="2">
-        <v>4.8220000000000001</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
@@ -4285,17 +4305,17 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
+      <c r="A241" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B241" s="3">
         <v>2021</v>
       </c>
       <c r="C241" s="2">
-        <v>0.22333333333333336</v>
+        <v>0.3</v>
       </c>
       <c r="D241" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
@@ -4313,37 +4333,158 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" s="1"/>
+      <c r="A243" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B243" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C243" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D243" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A244" s="1"/>
+      <c r="A244" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B244" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C244" s="2">
+        <v>0</v>
+      </c>
+      <c r="D244" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A245" s="1"/>
+      <c r="A245" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B245" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C245" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D245" s="2">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" s="1"/>
+      <c r="A246" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B246" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C246" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="D246" s="2">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" s="1"/>
+      <c r="A247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B247" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C247" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D247" s="2">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A248" s="1"/>
+      <c r="A248" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B248" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C248" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D248" s="2">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A249" s="1"/>
+      <c r="A249" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B249" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C249" s="2">
+        <v>6</v>
+      </c>
+      <c r="D249" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A250" s="1"/>
+      <c r="A250" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B250" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C250" s="2">
+        <v>1</v>
+      </c>
+      <c r="D250" s="2">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" s="1"/>
+      <c r="A251" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B251" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C251" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="D251" s="2">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A252" s="1"/>
+      <c r="A252" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B252" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C252" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D252" s="2">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A253" s="1"/>
+      <c r="A253" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B253" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C253" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="D253" s="2">
+        <v>1.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4352,20 +4493,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="170a3dc7-ecde-4c85-b711-1781140f65e4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="170a3dc7-ecde-4c85-b711-1781140f65e4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4604,14 +4745,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1525567-EE89-4EEE-82EE-FDC6792ABCE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBD46642-C4C7-4F32-A52D-2A4E275B13DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4624,6 +4757,14 @@
     <ds:schemaRef ds:uri="e57b8fe3-1221-4d4e-9419-2e191b8fa5ac"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1525567-EE89-4EEE-82EE-FDC6792ABCE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>